<commit_message>
Die Finale Version der App und des Workspaces, die restlichen Dokumente folgen in Kürze, ich bitte vielmals um Entschuldigung
</commit_message>
<xml_diff>
--- a/Planning-BauX/2.PM-Sheet.xlsx
+++ b/Planning-BauX/2.PM-Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armin\Desktop\project-proposal-baux\Planning-BauX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60E4F36-9000-47F0-B6DD-D94EC71FD97A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35F0CC2-E986-474B-9966-95ED3AF794E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,7 +102,7 @@
     <t>Djukic, Hamzic, Taha</t>
   </si>
   <si>
-    <t>Hamzic, Djukic</t>
+    <t>Hamzic</t>
   </si>
 </sst>
 </file>

</xml_diff>